<commit_message>
Final maintenance + auth system
</commit_message>
<xml_diff>
--- a/talkk_users.xlsx
+++ b/talkk_users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,6 +467,57 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Achu</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ashwinor0812@gmail.com</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$FdWQWR7qY0iQLMXR$bde4fd2a777f18096b4a1575d8bd892f2dce9041e4ed6dd3f7573c68f6fb26adc8274d46a0312448f77573885bd5df6073d4425328c177b6d0bd7e5a774561f9</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>testuser2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>test2@test.com</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>testpass</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ashw</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ashwinor000@gmail.com</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>scrypt:32768:8:1$ffvEDCcw7JImFPBH$c13c0b0eaead011e78a41f3fe2e2adca7b95f99a9ab2e4e1647942209d5dd2e009e7fcdb28d509f939de53ea09812cc33c550859bf5386dd002ac93aef5c6717</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>